<commit_message>
poke arm length change
</commit_message>
<xml_diff>
--- a/Poke Arm/Poke Arm Dims and Calcs (version 1).xlsx
+++ b/Poke Arm/Poke Arm Dims and Calcs (version 1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Centr\Documents\Mech-Peripherals\Poke Arm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\GitHub\Mech-Peripherals\Poke Arm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28D9A90-86EC-4FBC-829F-BD2E1F481917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5938BA53-68F2-40B3-B2C6-E038E16F61C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,12 +432,12 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -448,18 +448,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>60</v>
-      </c>
-      <c r="C2">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="G2">
         <v>9.81</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -473,7 +470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -486,14 +483,14 @@
       </c>
       <c r="D5">
         <f>C5/($B$2+$C$2)*1000</f>
-        <v>25.06143888888889</v>
+        <v>7.5184316666666673</v>
       </c>
       <c r="E5">
         <f>D5/$G$2*1000</f>
-        <v>2554.6828632914262</v>
+        <v>766.40485898742782</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -506,11 +503,11 @@
       </c>
       <c r="D6">
         <f>C6/($B$2+$C$2)*1000</f>
-        <v>2.7240694444444444</v>
+        <v>0.81722083333333329</v>
       </c>
       <c r="E6">
         <f>D6/$G$2*1000</f>
-        <v>277.68291992298106</v>
+        <v>83.304875976894323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>